<commit_message>
Itération 2 - Finale
</commit_message>
<xml_diff>
--- a/fichierPourTest/JeuDonnee.xlsx
+++ b/fichierPourTest/JeuDonnee.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A98EC3-19D5-4E63-92D2-43E772133655}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1849E252-FDD3-414E-BF10-D40EDCD99D07}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8628" yWindow="2940" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13872" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="283">
   <si>
     <t>grp</t>
   </si>
@@ -809,6 +809,66 @@
   </si>
   <si>
     <t>Frédéric</t>
+  </si>
+  <si>
+    <t>Fortier</t>
+  </si>
+  <si>
+    <t>Brodeur</t>
+  </si>
+  <si>
+    <t>Alphonse</t>
+  </si>
+  <si>
+    <t>Bussiere</t>
+  </si>
+  <si>
+    <t>Matthieu</t>
+  </si>
+  <si>
+    <t>Mouet</t>
+  </si>
+  <si>
+    <t>Amaury</t>
+  </si>
+  <si>
+    <t>Douffet</t>
+  </si>
+  <si>
+    <t>Estelle</t>
+  </si>
+  <si>
+    <t>Franchet</t>
+  </si>
+  <si>
+    <t>Mayhew</t>
+  </si>
+  <si>
+    <t>Compagnon</t>
+  </si>
+  <si>
+    <t>Gregoire</t>
+  </si>
+  <si>
+    <t>Boulé</t>
+  </si>
+  <si>
+    <t>Magnolia</t>
+  </si>
+  <si>
+    <t>Corbin</t>
+  </si>
+  <si>
+    <t>Dufresne</t>
+  </si>
+  <si>
+    <t>Lirienne</t>
+  </si>
+  <si>
+    <t>Françoise</t>
+  </si>
+  <si>
+    <t>Boivin</t>
   </si>
 </sst>
 </file>
@@ -1126,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="D137" sqref="D136:D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2591,6 +2651,127 @@
         <v>151</v>
       </c>
     </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>263</v>
+      </c>
+      <c r="B131" t="s">
+        <v>193</v>
+      </c>
+      <c r="C131" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>264</v>
+      </c>
+      <c r="B132" t="s">
+        <v>265</v>
+      </c>
+      <c r="C132" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>266</v>
+      </c>
+      <c r="B133" t="s">
+        <v>267</v>
+      </c>
+      <c r="C133" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>268</v>
+      </c>
+      <c r="B134" t="s">
+        <v>269</v>
+      </c>
+      <c r="C134" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>270</v>
+      </c>
+      <c r="B135" t="s">
+        <v>271</v>
+      </c>
+      <c r="C135" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>272</v>
+      </c>
+      <c r="B136" t="s">
+        <v>273</v>
+      </c>
+      <c r="C136" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>274</v>
+      </c>
+      <c r="B137" t="s">
+        <v>275</v>
+      </c>
+      <c r="C137" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>276</v>
+      </c>
+      <c r="B138" t="s">
+        <v>277</v>
+      </c>
+      <c r="C138" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>278</v>
+      </c>
+      <c r="B139" t="s">
+        <v>229</v>
+      </c>
+      <c r="C139" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>279</v>
+      </c>
+      <c r="B140" t="s">
+        <v>280</v>
+      </c>
+      <c r="C140" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>281</v>
+      </c>
+      <c r="B141" t="s">
+        <v>282</v>
+      </c>
+      <c r="C141" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout de la doc
</commit_message>
<xml_diff>
--- a/fichierPourTest/JeuDonnee.xlsx
+++ b/fichierPourTest/JeuDonnee.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1849E252-FDD3-414E-BF10-D40EDCD99D07}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="13872" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13875" yWindow="3390" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="286">
   <si>
     <t>grp</t>
   </si>
@@ -869,12 +868,21 @@
   </si>
   <si>
     <t>Boivin</t>
+  </si>
+  <si>
+    <t>Tiers-temps(prise en compte)</t>
+  </si>
+  <si>
+    <t>Tiers-temps(non pris en compte)</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -884,12 +892,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -904,8 +918,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1185,39 +1200,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E141"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="D137" sqref="D136:D137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1230,8 +1253,11 @@
       <c r="D2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1242,7 +1268,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1253,7 +1279,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1263,8 +1289,11 @@
       <c r="C5" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -1274,8 +1303,11 @@
       <c r="C6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1286,7 +1318,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -1296,8 +1328,11 @@
       <c r="C8" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1308,7 +1343,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -1319,7 +1354,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -1330,7 +1365,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -1341,7 +1376,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -1352,7 +1387,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1363,7 +1398,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -1374,7 +1409,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -1385,7 +1420,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -1396,7 +1431,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -1407,7 +1442,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -1418,7 +1453,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1428,8 +1463,11 @@
       <c r="C20" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -1440,7 +1478,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -1451,7 +1489,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -1462,7 +1500,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1473,7 +1511,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1484,7 +1522,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -1495,7 +1533,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1506,7 +1544,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -1517,7 +1555,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -1528,7 +1566,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -1542,7 +1580,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -1553,7 +1591,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -1564,7 +1602,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -1575,7 +1613,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -1586,7 +1624,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -1597,7 +1635,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -1608,7 +1646,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -1619,7 +1657,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -1630,7 +1668,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>112</v>
       </c>
@@ -1641,7 +1679,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -1652,7 +1690,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>114</v>
       </c>
@@ -1663,7 +1701,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -1674,7 +1712,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -1688,7 +1726,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>117</v>
       </c>
@@ -1699,7 +1737,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>118</v>
       </c>
@@ -1710,7 +1748,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -1721,7 +1759,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -1732,7 +1770,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -1743,7 +1781,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -1754,7 +1792,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>123</v>
       </c>
@@ -1765,7 +1803,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>124</v>
       </c>
@@ -1776,7 +1814,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>125</v>
       </c>
@@ -1787,7 +1825,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>126</v>
       </c>
@@ -1798,7 +1836,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>127</v>
       </c>
@@ -1809,7 +1847,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>128</v>
       </c>
@@ -1820,7 +1858,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>129</v>
       </c>
@@ -1831,7 +1869,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>130</v>
       </c>
@@ -1842,7 +1880,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>131</v>
       </c>
@@ -1853,7 +1891,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>132</v>
       </c>
@@ -1864,7 +1902,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>133</v>
       </c>
@@ -1875,7 +1913,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>134</v>
       </c>
@@ -1889,7 +1927,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>135</v>
       </c>
@@ -1900,7 +1938,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>136</v>
       </c>
@@ -1911,7 +1949,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>137</v>
       </c>
@@ -1922,7 +1960,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>138</v>
       </c>
@@ -1933,7 +1971,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>139</v>
       </c>
@@ -1944,7 +1982,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -1955,7 +1993,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>141</v>
       </c>
@@ -1966,7 +2004,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>142</v>
       </c>
@@ -1977,7 +2015,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -1988,7 +2026,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>144</v>
       </c>
@@ -1999,7 +2037,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>145</v>
       </c>
@@ -2010,7 +2048,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>146</v>
       </c>
@@ -2021,7 +2059,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>147</v>
       </c>
@@ -2032,7 +2070,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>148</v>
       </c>
@@ -2043,7 +2081,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>149</v>
       </c>
@@ -2054,7 +2092,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>159</v>
       </c>
@@ -2065,7 +2103,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>161</v>
       </c>
@@ -2076,7 +2114,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>163</v>
       </c>
@@ -2087,7 +2125,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>165</v>
       </c>
@@ -2098,7 +2136,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>167</v>
       </c>
@@ -2109,7 +2147,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>169</v>
       </c>
@@ -2120,7 +2158,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>171</v>
       </c>
@@ -2131,7 +2169,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>172</v>
       </c>
@@ -2142,7 +2180,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -2153,7 +2191,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>176</v>
       </c>
@@ -2164,7 +2202,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>178</v>
       </c>
@@ -2175,7 +2213,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>180</v>
       </c>
@@ -2186,7 +2224,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>182</v>
       </c>
@@ -2197,7 +2235,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>184</v>
       </c>
@@ -2211,7 +2249,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>186</v>
       </c>
@@ -2222,7 +2260,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>188</v>
       </c>
@@ -2233,7 +2271,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>190</v>
       </c>
@@ -2244,7 +2282,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>192</v>
       </c>
@@ -2255,7 +2293,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>194</v>
       </c>
@@ -2266,7 +2304,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>196</v>
       </c>
@@ -2277,7 +2315,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>198</v>
       </c>
@@ -2288,7 +2326,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>200</v>
       </c>
@@ -2299,7 +2337,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>202</v>
       </c>
@@ -2310,7 +2348,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>203</v>
       </c>
@@ -2321,7 +2359,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>205</v>
       </c>
@@ -2332,7 +2370,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>207</v>
       </c>
@@ -2343,7 +2381,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>209</v>
       </c>
@@ -2354,7 +2392,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>211</v>
       </c>
@@ -2365,7 +2403,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>213</v>
       </c>
@@ -2376,7 +2414,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>215</v>
       </c>
@@ -2387,7 +2425,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>216</v>
       </c>
@@ -2398,7 +2436,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>218</v>
       </c>
@@ -2409,7 +2447,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>220</v>
       </c>
@@ -2420,7 +2458,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -2431,7 +2469,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -2442,7 +2480,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>226</v>
       </c>
@@ -2453,7 +2491,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -2464,7 +2502,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>230</v>
       </c>
@@ -2475,7 +2513,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -2486,7 +2524,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>234</v>
       </c>
@@ -2497,7 +2535,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>235</v>
       </c>
@@ -2508,7 +2546,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>237</v>
       </c>
@@ -2519,7 +2557,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>239</v>
       </c>
@@ -2530,7 +2568,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>241</v>
       </c>
@@ -2541,7 +2579,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>243</v>
       </c>
@@ -2552,7 +2590,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>245</v>
       </c>
@@ -2563,7 +2601,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>247</v>
       </c>
@@ -2574,7 +2612,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>249</v>
       </c>
@@ -2585,7 +2623,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>251</v>
       </c>
@@ -2596,7 +2634,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>253</v>
       </c>
@@ -2607,7 +2645,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>255</v>
       </c>
@@ -2618,7 +2656,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>257</v>
       </c>
@@ -2629,7 +2667,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>259</v>
       </c>
@@ -2640,7 +2678,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>261</v>
       </c>
@@ -2651,7 +2689,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>263</v>
       </c>
@@ -2662,7 +2700,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>264</v>
       </c>
@@ -2673,7 +2711,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>266</v>
       </c>
@@ -2684,7 +2722,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>268</v>
       </c>
@@ -2695,7 +2733,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>270</v>
       </c>
@@ -2706,7 +2744,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>272</v>
       </c>
@@ -2717,7 +2755,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>274</v>
       </c>
@@ -2728,7 +2766,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>276</v>
       </c>
@@ -2739,7 +2777,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>278</v>
       </c>
@@ -2750,7 +2788,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>279</v>
       </c>
@@ -2761,7 +2799,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>281</v>
       </c>

</xml_diff>

<commit_message>
Correction bug import Excel
</commit_message>
<xml_diff>
--- a/fichierPourTest/JeuDonnee.xlsx
+++ b/fichierPourTest/JeuDonnee.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="286">
   <si>
     <t>grp</t>
   </si>
@@ -1204,7 +1204,7 @@
   <dimension ref="A1:G141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,9 +1253,6 @@
       <c r="D2" t="s">
         <v>157</v>
       </c>
-      <c r="G2" t="s">
-        <v>285</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>